<commit_message>
Update Matriz de comunicação.xlsx
</commit_message>
<xml_diff>
--- a/Matriz de Comunicacao/Matriz de comunicação.xlsx
+++ b/Matriz de Comunicacao/Matriz de comunicação.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gestao-de-Portfolios\Matriz de Comunicacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F01A456-9867-4639-90AB-40270FDB7252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3181E8-DBFA-4D9B-8987-5671A8101732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{847C3544-8264-4759-A5F4-B4FD06DAD307}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="150">
   <si>
     <t>IDENTIFICAÇÃO E EXPECTATIVAS DAS PARTES INTERESSADAS</t>
   </si>
@@ -170,18 +170,6 @@
     <t>Uma vez</t>
   </si>
   <si>
-    <t>Documento de requisitos elaborado</t>
-  </si>
-  <si>
-    <t>Reunião Presencial/E-mail</t>
-  </si>
-  <si>
-    <t>Aceite de Requisitos</t>
-  </si>
-  <si>
-    <t>Aceitação do documento de requisitos</t>
-  </si>
-  <si>
     <t>Cliente</t>
   </si>
   <si>
@@ -333,9 +321,6 @@
 Através desses registros de informações serão levantadas as informações necessárias para levantamento de indicadores, e status do portfólio.  </t>
   </si>
   <si>
-    <t>Analista de Negócios</t>
-  </si>
-  <si>
     <t>Gerente de Portfólio</t>
   </si>
   <si>
@@ -357,55 +342,10 @@
     <t>Início do portfólio</t>
   </si>
   <si>
-    <t>Levantamento de Requisitos</t>
-  </si>
-  <si>
-    <t>Analista de Negócios, Time do Cliente</t>
-  </si>
-  <si>
-    <t>Extração de requisitos, escopo inicial, documentos de apoio</t>
-  </si>
-  <si>
-    <t>Documentação dos requisitos funcionais e não funcionais</t>
-  </si>
-  <si>
-    <t>Definição e documentação dos requisitos</t>
-  </si>
-  <si>
-    <t>Validação de Requisitos Interno</t>
-  </si>
-  <si>
     <t>Time de Portfólio</t>
   </si>
   <si>
-    <t>Apresentação dos requisitos para validação técnica</t>
-  </si>
-  <si>
-    <t>Validar requisitos e ajustar conforme necessário</t>
-  </si>
-  <si>
     <t>Uma vez ou até definição</t>
-  </si>
-  <si>
-    <t>Validação de Requisitos Externo</t>
-  </si>
-  <si>
-    <t>Analista de Negócios, Cliente</t>
-  </si>
-  <si>
-    <t>Documento de Requisitos</t>
-  </si>
-  <si>
-    <t>Apresentação dos requisitos revisados ao cliente</t>
-  </si>
-  <si>
-    <t>Alinhar expectativas do cliente com o que será desenvolvido</t>
-  </si>
-  <si>
-    <t>Base para desenvolvimento do sistema</t>
-  </si>
-  <si>
-    <t>E-mail/Reunião Presencial</t>
   </si>
   <si>
     <t>Definição de Arquitetura</t>
@@ -753,17 +693,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -780,54 +723,23 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Segoe UI"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -854,17 +766,45 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color theme="1"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-      </border>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -880,24 +820,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1074E750-66B9-436D-98DF-A0EA80D62937}" name="Tabela5" displayName="Tabela5" ref="B26:I45" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="10" tableBorderDxfId="11">
-  <autoFilter ref="B26:I45" xr:uid="{1074E750-66B9-436D-98DF-A0EA80D62937}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1074E750-66B9-436D-98DF-A0EA80D62937}" name="Tabela5" displayName="Tabela5" ref="B26:I41" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
+  <autoFilter ref="B26:I41" xr:uid="{1074E750-66B9-436D-98DF-A0EA80D62937}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C0C5CD48-1555-4286-83F3-9F266B7C19E2}" name="Evento" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{989788F2-3E1B-4852-8DB4-86AD86290F7F}" name="Participantes" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{FA8DC587-17A1-4EE5-BD1A-F7BA216C4DE4}" name="Informações e documentos" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{6549A435-DD60-430B-A345-5EF6470F28FB}" name="O que precisa ser comunicado ?" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{70F1B56A-C265-421F-9702-98D3587969E6}" name="Motivo" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{91E4FF2A-98C2-476E-9C98-8A5FF28655F8}" name="Método de Comunicação" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{C470862E-C889-4089-8507-7A34828848DE}" name="Responsável" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{9165AB75-C439-494A-831F-3A9014E19ECA}" name="Frequencia" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{C0C5CD48-1555-4286-83F3-9F266B7C19E2}" name="Evento" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{989788F2-3E1B-4852-8DB4-86AD86290F7F}" name="Participantes" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{FA8DC587-17A1-4EE5-BD1A-F7BA216C4DE4}" name="Informações e documentos" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{6549A435-DD60-430B-A345-5EF6470F28FB}" name="O que precisa ser comunicado ?" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{70F1B56A-C265-421F-9702-98D3587969E6}" name="Motivo" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{91E4FF2A-98C2-476E-9C98-8A5FF28655F8}" name="Método de Comunicação" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{C470862E-C889-4089-8507-7A34828848DE}" name="Responsável" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{9165AB75-C439-494A-831F-3A9014E19ECA}" name="Frequencia" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -1193,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACDF89A-10DA-45B9-91D4-DB36A460FEF4}">
-  <dimension ref="B4:I45"/>
+  <dimension ref="B4:I41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -1214,16 +1154,16 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C5" s="5"/>
@@ -1253,20 +1193,20 @@
       <c r="G6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7" spans="2:9" ht="33.6" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>8</v>
@@ -1277,20 +1217,20 @@
       <c r="G7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="2:9" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="H7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="18"/>
+    </row>
+    <row r="8" spans="2:9" ht="33.6" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>8</v>
@@ -1299,22 +1239,22 @@
         <v>9</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="2:9" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="2:9" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>9</v>
@@ -1323,22 +1263,22 @@
         <v>8</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="I9" s="8"/>
+        <v>57</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="2:9" ht="33.6" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>11</v>
@@ -1347,16 +1287,16 @@
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="2:9" ht="33.6" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>12</v>
@@ -1373,20 +1313,20 @@
       <c r="G11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="2:9" ht="67.2" x14ac:dyDescent="0.3">
+      <c r="H11" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="18"/>
+    </row>
+    <row r="12" spans="2:9" ht="50.4" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>9</v>
@@ -1395,22 +1335,22 @@
         <v>8</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" s="18"/>
+    </row>
+    <row r="13" spans="2:9" ht="67.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="2:9" ht="84" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>8</v>
@@ -1419,22 +1359,22 @@
         <v>9</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" spans="2:9" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="2:9" ht="84" x14ac:dyDescent="0.3">
-      <c r="B14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>8</v>
@@ -1443,12 +1383,12 @@
         <v>9</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="I14" s="8"/>
+        <v>77</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" s="18"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
@@ -1457,8 +1397,8 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="8"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
@@ -1467,8 +1407,8 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="8"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="18"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
@@ -1477,8 +1417,8 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="8"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="18"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
@@ -1487,604 +1427,505 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="8"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="18"/>
     </row>
     <row r="19" spans="2:9" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
     </row>
     <row r="20" spans="2:9" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
     </row>
     <row r="21" spans="2:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+    </row>
+    <row r="23" spans="2:9" ht="67.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="2:9" ht="321.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+    </row>
+    <row r="25" spans="2:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-    </row>
-    <row r="23" spans="2:9" ht="67.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="2:9" ht="321.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-    </row>
-    <row r="25" spans="2:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="13" t="s">
+      <c r="E27" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G31" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-    </row>
-    <row r="26" spans="2:9" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="B26" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="H26" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I26" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B27" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="I27" s="16" t="s">
+      <c r="H31" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B32" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G32" s="7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="28" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B28" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H28" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="I28" s="16" t="s">
+      <c r="H32" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B33" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I34" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B29" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D29" s="16" t="s">
+    <row r="35" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B36" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B37" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="D39" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G41" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="F29" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="I29" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H30" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="I30" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="E31" s="16" t="s">
+      <c r="H41" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I41" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I31" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G32" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="H32" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="I32" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="I33" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="G34" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="I34" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="G35" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="H35" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="I35" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B36" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="G36" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="H36" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="I36" s="16" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B37" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="H37" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="I37" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="H38" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="I38" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="G39" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="H39" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="I39" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B40" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D40" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="F40" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="G40" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="H40" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="I40" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B41" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="F41" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="G41" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="H41" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="I41" s="16" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="F42" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G42" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="H42" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="I42" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="H43" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I43" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C44" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E44" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="F44" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="G44" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="H44" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="I44" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="E45" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="G45" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="H45" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="I45" s="16" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
     <mergeCell ref="B4:I4"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:I25"/>
@@ -2101,11 +1942,6 @@
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>